<commit_message>
20 cases completed for StJudes
</commit_message>
<xml_diff>
--- a/stJude/src/main/resources/StJudePatientReferralsExpectedElements.xlsx
+++ b/stJude/src/main/resources/StJudePatientReferralsExpectedElements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamin\IdeaProjects\AutomationFramework_Team3\stJude\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F880488-D9AF-46A8-A02A-FED0A97E968F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B01344-FAC9-46F7-83BB-B26F2A4ED5E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="825" firstSheet="5" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contactUsTitle" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,16 @@
     <sheet name="donateNowTitle" sheetId="3" r:id="rId3"/>
     <sheet name="aboutUsLinks" sheetId="4" r:id="rId4"/>
     <sheet name="searchResultsTitle" sheetId="5" r:id="rId5"/>
+    <sheet name="bodyLinksCount" sheetId="6" r:id="rId6"/>
+    <sheet name="bodyTabsTitles" sheetId="7" r:id="rId7"/>
+    <sheet name="forReferringPhysicians" sheetId="9" r:id="rId8"/>
+    <sheet name="clinicalTrialsTitle" sheetId="10" r:id="rId9"/>
+    <sheet name="acceptanceRequirementsText" sheetId="12" r:id="rId10"/>
+    <sheet name="contactFormUrl" sheetId="14" r:id="rId11"/>
+    <sheet name="socialMediaIcons" sheetId="15" r:id="rId12"/>
+    <sheet name="partnersLinks" sheetId="13" r:id="rId13"/>
+    <sheet name="siteMapTitle" sheetId="16" r:id="rId14"/>
+    <sheet name="linkingPolicyTitle" sheetId="17" r:id="rId15"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Contact us at St. Jude Children’s Research Hospital - St. Jude Children’s Research Hospital</t>
   </si>
@@ -41,16 +51,98 @@
   </si>
   <si>
     <t>Search Results - St. Jude Children’s Research Hospital</t>
+  </si>
+  <si>
+    <t>https://www.stjude.org/patient-referrals/seek-treatment.html</t>
+  </si>
+  <si>
+    <t>https://www.stjude.org/disease.html</t>
+  </si>
+  <si>
+    <t>https://www.stjude.org/treatment/patient-resources/before-arrival/what-to-bring.html</t>
+  </si>
+  <si>
+    <t>https://www.stjude.org/patient-referrals/seek-treatment/taking-part-in-clinical-research.html</t>
+  </si>
+  <si>
+    <t>https://www.stjude.org/patient-referrals/refer-a-patient.html</t>
+  </si>
+  <si>
+    <t>https://www.stjude.org/patient-referrals/refer-a-patient/how-to-request-consult.html</t>
+  </si>
+  <si>
+    <t>https://www.stjude.org/patient-referrals/refer-a-patient/transitioning-your-patient-to-st-jude.html</t>
+  </si>
+  <si>
+    <t>https://www.stjude.org/patient-referrals/refer-a-patient/what-to-tell-your-patient.html</t>
+  </si>
+  <si>
+    <t>https://www.stjude.org/patient-referrals/refer-a-patient/monitoring-your-patients-progress.html</t>
+  </si>
+  <si>
+    <t>Clinical Trials - St. Jude Children’s Research Hospital</t>
+  </si>
+  <si>
+    <t>To be accepted at St. Jude, children must be eligible for one of our open clinical trials or meet one of the additional criteria listed below. They must also be referred by a physician or qualified medical professional.
+Requirements for acceptance to a St. Jude clinical trial include:
+Age range
+Type and stage of disease
+Other medical criteria including organ function, blood values, performance scores, etc.
+Some trials only accept children if they have not yet begun treatment.</t>
+  </si>
+  <si>
+    <t>https://hospital.stjude.org/apps/forms/fb/physician-referral-form/</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/stjude</t>
+  </si>
+  <si>
+    <t>https://twitter.com/StJude</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/stjude/</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/user/MyStJude</t>
+  </si>
+  <si>
+    <t>https://health.usnews.com/best-hospitals/area/tn/st-jude-childrens-research-hospital-6520815</t>
+  </si>
+  <si>
+    <t>https://www.nursingworld.org/organizational-programs/magnet/</t>
+  </si>
+  <si>
+    <t>https://www.cancer.gov/research/infrastructure/cancer-centers</t>
+  </si>
+  <si>
+    <t>https://www.give.org/charity-reviews/national/Other/ALSAC-St.-Jude-Childrens-Research-Hospital-in-Memphis-tn-2903</t>
+  </si>
+  <si>
+    <t>https://www.charitynavigator.org/index.cfm?bay=search.summary&amp;orgid=12847</t>
+  </si>
+  <si>
+    <t>Site Map - St. Jude Children’s Research Hospital</t>
+  </si>
+  <si>
+    <t>Linking Policy - St. Jude Children’s Research Hospital</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -73,13 +165,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -374,13 +475,196 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD00DBD1-8EBC-467B-AC0A-B43CF02A6AF5}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="176.53125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="87" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5248EE9-2D22-4E2E-BFF9-F423BA286AA4}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="60.1328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{AB7D57A8-3F1C-4A72-AB69-3C1BCF5DD34D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D7DF95A-0710-4D73-8D8E-F8AA22A4C7E0}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="45.46484375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{2FA99D8B-F894-4316-A30E-BD202FDD517A}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{6AA92C71-8549-4824-994E-D221D5B9876D}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{9A9BBA38-B623-473C-B3ED-395BF3FE3F41}"/>
+    <hyperlink ref="A4" r:id="rId4" xr:uid="{9955504A-0EED-4ED3-B241-F0EFD6E77E06}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E01987A-010A-4D01-BF4B-373EE4F83086}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="90.9296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{648CF649-D6FA-4A98-A598-BD112FD633F1}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{50705540-DA33-469F-937E-41057A1E57A2}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{54F43D23-926E-41A1-B0A7-8016F7928F3E}"/>
+    <hyperlink ref="A4" r:id="rId4" xr:uid="{92551B50-74C4-46C4-9E0E-D923177EA66A}"/>
+    <hyperlink ref="A5" r:id="rId5" xr:uid="{8D89B8DD-3AAC-431A-A0A6-860E34D24D80}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E9F4AB6-776D-43BF-AC35-B3FA318C7C00}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B27706F5-0DE2-4F17-9A01-12DFA7435E6C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="54.265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{137C3E6C-8A4B-4062-A841-E803624B8A75}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="56" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
@@ -396,9 +680,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3AAFA4B-4048-4584-9B9F-2A1CA37B3FFF}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="77.46484375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
@@ -432,9 +721,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99247131-63BC-4E41-820B-60EC733264D2}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="54.265625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
@@ -444,4 +736,137 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86F9504A-5C87-42C0-8E81-CD3BDD102ED2}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFBE4D5C-0935-4F3E-80F2-823D93B036EB}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="90.9296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{24BEFE50-A00E-449B-9FBA-CBF0CE222E7A}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{D8B718A3-E5B5-4CAD-99AD-67CC8C381760}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{89E6ECE7-052B-4822-9AD0-9939405AAE27}"/>
+    <hyperlink ref="A1" r:id="rId4" xr:uid="{6286A5F9-6933-41A7-B9A2-36175DE241CC}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FDE3513-AFB4-4247-8489-C31FC987E06D}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="89.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{C16971F0-EC73-487E-882C-EE998605F6AB}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{EED1B207-C4F9-4343-91DE-57B01E844D38}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{38729F59-86E6-44FF-8F39-5EF5833F79E5}"/>
+    <hyperlink ref="A4" r:id="rId4" xr:uid="{5CE0E1A0-7212-4F95-88B8-8F1EAC9D901E}"/>
+    <hyperlink ref="A5" r:id="rId5" xr:uid="{20541A57-E45C-49D3-8543-B41CC87D4472}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2203A5C5-B87E-4187-B060-F7BDA74549FA}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="53.19921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>